<commit_message>
cap nhat file da sua
</commit_message>
<xml_diff>
--- a/ketqua.xlsx
+++ b/ketqua.xlsx
@@ -539,28 +539,27 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lỗi: Message: no such element: Unable to locate element: {"method":"css selector","selector":"[id="btnSearch"]"}
-  (Session info: chrome=137.0.7151.120); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+          <t xml:space="preserve">Lỗi: Message: 
 Stacktrace:
-	GetHandleVerifier [0x0x443b03+62899]
-	GetHandleVerifier [0x0x443b44+62964]
-	(No symbol) [0x0x2710f3]
-	(No symbol) [0x0x2b980e]
-	(No symbol) [0x0x2b9bab]
-	(No symbol) [0x0x3025c2]
-	(No symbol) [0x0x2de554]
-	(No symbol) [0x0x2ffd81]
-	(No symbol) [0x0x2de306]
-	(No symbol) [0x0x2ad670]
-	(No symbol) [0x0x2ae4e4]
-	GetHandleVerifier [0x0x6a4793+2556483]
-	GetHandleVerifier [0x0x69fd02+2537394]
-	GetHandleVerifier [0x0x46a2fa+220586]
-	GetHandleVerifier [0x0x45aae8+157080]
-	GetHandleVerifier [0x0x46141d+184013]
-	GetHandleVerifier [0x0x44ba68+95512]
-	GetHandleVerifier [0x0x44bc10+95936]
-	GetHandleVerifier [0x0x436b5a+9738]
+	GetHandleVerifier [0x0x8c3b03+62899]
+	GetHandleVerifier [0x0x8c3b44+62964]
+	(No symbol) [0x0x6f10f3]
+	(No symbol) [0x0x73980e]
+	(No symbol) [0x0x739bab]
+	(No symbol) [0x0x7825c2]
+	(No symbol) [0x0x75e554]
+	(No symbol) [0x0x77fd81]
+	(No symbol) [0x0x75e306]
+	(No symbol) [0x0x72d670]
+	(No symbol) [0x0x72e4e4]
+	GetHandleVerifier [0x0xb24793+2556483]
+	GetHandleVerifier [0x0xb1fd02+2537394]
+	GetHandleVerifier [0x0x8ea2fa+220586]
+	GetHandleVerifier [0x0x8daae8+157080]
+	GetHandleVerifier [0x0x8e141d+184013]
+	GetHandleVerifier [0x0x8cba68+95512]
+	GetHandleVerifier [0x0x8cbc10+95936]
+	GetHandleVerifier [0x0x8b6b5a+9738]
 	BaseThreadInitThunk [0x0x75977ba9+25]
 	RtlInitializeExceptionChain [0x0x770ac3ab+107]
 	RtlClearBits [0x0x770ac32f+191]
@@ -586,28 +585,27 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lỗi: Message: no such element: Unable to locate element: {"method":"css selector","selector":"[id="btnSearch"]"}
-  (Session info: chrome=137.0.7151.120); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+          <t xml:space="preserve">Lỗi: Message: 
 Stacktrace:
-	GetHandleVerifier [0x0x443b03+62899]
-	GetHandleVerifier [0x0x443b44+62964]
-	(No symbol) [0x0x2710f3]
-	(No symbol) [0x0x2b980e]
-	(No symbol) [0x0x2b9bab]
-	(No symbol) [0x0x3025c2]
-	(No symbol) [0x0x2de554]
-	(No symbol) [0x0x2ffd81]
-	(No symbol) [0x0x2de306]
-	(No symbol) [0x0x2ad670]
-	(No symbol) [0x0x2ae4e4]
-	GetHandleVerifier [0x0x6a4793+2556483]
-	GetHandleVerifier [0x0x69fd02+2537394]
-	GetHandleVerifier [0x0x46a2fa+220586]
-	GetHandleVerifier [0x0x45aae8+157080]
-	GetHandleVerifier [0x0x46141d+184013]
-	GetHandleVerifier [0x0x44ba68+95512]
-	GetHandleVerifier [0x0x44bc10+95936]
-	GetHandleVerifier [0x0x436b5a+9738]
+	GetHandleVerifier [0x0x8c3b03+62899]
+	GetHandleVerifier [0x0x8c3b44+62964]
+	(No symbol) [0x0x6f10f3]
+	(No symbol) [0x0x73980e]
+	(No symbol) [0x0x739bab]
+	(No symbol) [0x0x7825c2]
+	(No symbol) [0x0x75e554]
+	(No symbol) [0x0x77fd81]
+	(No symbol) [0x0x75e306]
+	(No symbol) [0x0x72d670]
+	(No symbol) [0x0x72e4e4]
+	GetHandleVerifier [0x0xb24793+2556483]
+	GetHandleVerifier [0x0xb1fd02+2537394]
+	GetHandleVerifier [0x0x8ea2fa+220586]
+	GetHandleVerifier [0x0x8daae8+157080]
+	GetHandleVerifier [0x0x8e141d+184013]
+	GetHandleVerifier [0x0x8cba68+95512]
+	GetHandleVerifier [0x0x8cbc10+95936]
+	GetHandleVerifier [0x0x8b6b5a+9738]
 	BaseThreadInitThunk [0x0x75977ba9+25]
 	RtlInitializeExceptionChain [0x0x770ac3ab+107]
 	RtlClearBits [0x0x770ac32f+191]
@@ -633,28 +631,27 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lỗi: Message: no such element: Unable to locate element: {"method":"css selector","selector":"[id="btnSearch"]"}
-  (Session info: chrome=137.0.7151.120); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+          <t xml:space="preserve">Lỗi: Message: 
 Stacktrace:
-	GetHandleVerifier [0x0x443b03+62899]
-	GetHandleVerifier [0x0x443b44+62964]
-	(No symbol) [0x0x2710f3]
-	(No symbol) [0x0x2b980e]
-	(No symbol) [0x0x2b9bab]
-	(No symbol) [0x0x3025c2]
-	(No symbol) [0x0x2de554]
-	(No symbol) [0x0x2ffd81]
-	(No symbol) [0x0x2de306]
-	(No symbol) [0x0x2ad670]
-	(No symbol) [0x0x2ae4e4]
-	GetHandleVerifier [0x0x6a4793+2556483]
-	GetHandleVerifier [0x0x69fd02+2537394]
-	GetHandleVerifier [0x0x46a2fa+220586]
-	GetHandleVerifier [0x0x45aae8+157080]
-	GetHandleVerifier [0x0x46141d+184013]
-	GetHandleVerifier [0x0x44ba68+95512]
-	GetHandleVerifier [0x0x44bc10+95936]
-	GetHandleVerifier [0x0x436b5a+9738]
+	GetHandleVerifier [0x0x8c3b03+62899]
+	GetHandleVerifier [0x0x8c3b44+62964]
+	(No symbol) [0x0x6f10f3]
+	(No symbol) [0x0x73980e]
+	(No symbol) [0x0x739bab]
+	(No symbol) [0x0x7825c2]
+	(No symbol) [0x0x75e554]
+	(No symbol) [0x0x77fd81]
+	(No symbol) [0x0x75e306]
+	(No symbol) [0x0x72d670]
+	(No symbol) [0x0x72e4e4]
+	GetHandleVerifier [0x0xb24793+2556483]
+	GetHandleVerifier [0x0xb1fd02+2537394]
+	GetHandleVerifier [0x0x8ea2fa+220586]
+	GetHandleVerifier [0x0x8daae8+157080]
+	GetHandleVerifier [0x0x8e141d+184013]
+	GetHandleVerifier [0x0x8cba68+95512]
+	GetHandleVerifier [0x0x8cbc10+95936]
+	GetHandleVerifier [0x0x8b6b5a+9738]
 	BaseThreadInitThunk [0x0x75977ba9+25]
 	RtlInitializeExceptionChain [0x0x770ac3ab+107]
 	RtlClearBits [0x0x770ac32f+191]
@@ -680,7 +677,31 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Không hỗ trợ URL này</t>
+          <t xml:space="preserve">Lỗi: Message: 
+Stacktrace:
+	GetHandleVerifier [0x0x8c3b03+62899]
+	GetHandleVerifier [0x0x8c3b44+62964]
+	(No symbol) [0x0x6f10f3]
+	(No symbol) [0x0x73980e]
+	(No symbol) [0x0x739bab]
+	(No symbol) [0x0x7825c2]
+	(No symbol) [0x0x75e554]
+	(No symbol) [0x0x77fd81]
+	(No symbol) [0x0x75e306]
+	(No symbol) [0x0x72d670]
+	(No symbol) [0x0x72e4e4]
+	GetHandleVerifier [0x0xb24793+2556483]
+	GetHandleVerifier [0x0xb1fd02+2537394]
+	GetHandleVerifier [0x0x8ea2fa+220586]
+	GetHandleVerifier [0x0x8daae8+157080]
+	GetHandleVerifier [0x0x8e141d+184013]
+	GetHandleVerifier [0x0x8cba68+95512]
+	GetHandleVerifier [0x0x8cbc10+95936]
+	GetHandleVerifier [0x0x8b6b5a+9738]
+	BaseThreadInitThunk [0x0x75977ba9+25]
+	RtlInitializeExceptionChain [0x0x770ac3ab+107]
+	RtlClearBits [0x0x770ac32f+191]
+</t>
         </is>
       </c>
     </row>
@@ -702,7 +723,31 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Không hỗ trợ URL này</t>
+          <t xml:space="preserve">Lỗi: Message: 
+Stacktrace:
+	GetHandleVerifier [0x0x8c3b03+62899]
+	GetHandleVerifier [0x0x8c3b44+62964]
+	(No symbol) [0x0x6f10f3]
+	(No symbol) [0x0x73980e]
+	(No symbol) [0x0x739bab]
+	(No symbol) [0x0x7825c2]
+	(No symbol) [0x0x75e554]
+	(No symbol) [0x0x77fd81]
+	(No symbol) [0x0x75e306]
+	(No symbol) [0x0x72d670]
+	(No symbol) [0x0x72e4e4]
+	GetHandleVerifier [0x0xb24793+2556483]
+	GetHandleVerifier [0x0xb1fd02+2537394]
+	GetHandleVerifier [0x0x8ea2fa+220586]
+	GetHandleVerifier [0x0x8daae8+157080]
+	GetHandleVerifier [0x0x8e141d+184013]
+	GetHandleVerifier [0x0x8cba68+95512]
+	GetHandleVerifier [0x0x8cbc10+95936]
+	GetHandleVerifier [0x0x8b6b5a+9738]
+	BaseThreadInitThunk [0x0x75977ba9+25]
+	RtlInitializeExceptionChain [0x0x770ac3ab+107]
+	RtlClearBits [0x0x770ac32f+191]
+</t>
         </is>
       </c>
     </row>
@@ -724,7 +769,31 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Không hỗ trợ URL này</t>
+          <t xml:space="preserve">Lỗi: Message: 
+Stacktrace:
+	GetHandleVerifier [0x0x8c3b03+62899]
+	GetHandleVerifier [0x0x8c3b44+62964]
+	(No symbol) [0x0x6f10f3]
+	(No symbol) [0x0x73980e]
+	(No symbol) [0x0x739bab]
+	(No symbol) [0x0x7825c2]
+	(No symbol) [0x0x75e554]
+	(No symbol) [0x0x77fd81]
+	(No symbol) [0x0x75e306]
+	(No symbol) [0x0x72d670]
+	(No symbol) [0x0x72e4e4]
+	GetHandleVerifier [0x0xb24793+2556483]
+	GetHandleVerifier [0x0xb1fd02+2537394]
+	GetHandleVerifier [0x0x8ea2fa+220586]
+	GetHandleVerifier [0x0x8daae8+157080]
+	GetHandleVerifier [0x0x8e141d+184013]
+	GetHandleVerifier [0x0x8cba68+95512]
+	GetHandleVerifier [0x0x8cbc10+95936]
+	GetHandleVerifier [0x0x8b6b5a+9738]
+	BaseThreadInitThunk [0x0x75977ba9+25]
+	RtlInitializeExceptionChain [0x0x770ac3ab+107]
+	RtlClearBits [0x0x770ac32f+191]
+</t>
         </is>
       </c>
     </row>

</xml_diff>